<commit_message>
user login from oauth 2.0 provider done
</commit_message>
<xml_diff>
--- a/config_dummy.xlsx
+++ b/config_dummy.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
   <si>
     <t>flaskSecret</t>
   </si>
@@ -105,6 +105,21 @@
   </si>
   <si>
     <t>outagesFetchUrl</t>
+  </si>
+  <si>
+    <t>oauth_app_client_id</t>
+  </si>
+  <si>
+    <t>oauth_app_client_secret</t>
+  </si>
+  <si>
+    <t>oauth_provider_discovery_url</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>secret</t>
   </si>
 </sst>
 </file>
@@ -485,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,6 +693,30 @@
         <v>25</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -698,9 +737,10 @@
     <hyperlink ref="B21" r:id="rId13"/>
     <hyperlink ref="B22:B23" r:id="rId14" display="http://google.com"/>
     <hyperlink ref="B20" r:id="rId15"/>
+    <hyperlink ref="B26" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
app prefix config variable
</commit_message>
<xml_diff>
--- a/config_dummy.xlsx
+++ b/config_dummy.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
   <si>
     <t>flaskSecret</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>secret</t>
+  </si>
+  <si>
+    <t>appPrefix</t>
+  </si>
+  <si>
+    <t>/mis_dashboard</t>
   </si>
 </sst>
 </file>
@@ -500,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,15 +544,15 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>3</v>
@@ -554,7 +560,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>3</v>
@@ -562,7 +568,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
@@ -570,7 +576,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>3</v>
@@ -578,7 +584,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>3</v>
@@ -586,7 +592,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>3</v>
@@ -594,7 +600,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>3</v>
@@ -602,7 +608,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>3</v>
@@ -610,7 +616,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>3</v>
@@ -618,7 +624,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>3</v>
@@ -626,7 +632,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>3</v>
@@ -634,7 +640,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>3</v>
@@ -642,23 +648,23 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>3</v>
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>3</v>
@@ -666,7 +672,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>3</v>
@@ -674,7 +680,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>3</v>
@@ -682,7 +688,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>3</v>
@@ -690,7 +696,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>3</v>
@@ -698,46 +704,54 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" t="s">
-        <v>30</v>
+        <v>25</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1"/>
-    <hyperlink ref="B5" r:id="rId2"/>
-    <hyperlink ref="B6" r:id="rId3"/>
-    <hyperlink ref="B7" r:id="rId4"/>
-    <hyperlink ref="B8" r:id="rId5"/>
-    <hyperlink ref="B9" r:id="rId6"/>
-    <hyperlink ref="B10" r:id="rId7"/>
-    <hyperlink ref="B11" r:id="rId8"/>
-    <hyperlink ref="B12:B15" r:id="rId9" display="http://google.com"/>
-    <hyperlink ref="B16" r:id="rId10"/>
-    <hyperlink ref="B18" r:id="rId11"/>
-    <hyperlink ref="B19" r:id="rId12"/>
-    <hyperlink ref="B21" r:id="rId13"/>
-    <hyperlink ref="B22:B23" r:id="rId14" display="http://google.com"/>
-    <hyperlink ref="B20" r:id="rId15"/>
-    <hyperlink ref="B26" r:id="rId16"/>
+    <hyperlink ref="B5" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId2"/>
+    <hyperlink ref="B7" r:id="rId3"/>
+    <hyperlink ref="B8" r:id="rId4"/>
+    <hyperlink ref="B9" r:id="rId5"/>
+    <hyperlink ref="B10" r:id="rId6"/>
+    <hyperlink ref="B11" r:id="rId7"/>
+    <hyperlink ref="B12" r:id="rId8"/>
+    <hyperlink ref="B13:B16" r:id="rId9" display="http://google.com"/>
+    <hyperlink ref="B17" r:id="rId10"/>
+    <hyperlink ref="B19" r:id="rId11"/>
+    <hyperlink ref="B20" r:id="rId12"/>
+    <hyperlink ref="B22" r:id="rId13"/>
+    <hyperlink ref="B23:B24" r:id="rId14" display="http://google.com"/>
+    <hyperlink ref="B21" r:id="rId15"/>
+    <hyperlink ref="B27" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId17"/>

</xml_diff>

<commit_message>
config dummy updated for monthly report
</commit_message>
<xml_diff>
--- a/config_dummy.xlsx
+++ b/config_dummy.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nagasudhir\Documents\Python Projects\mis_software\wrldc_mis_flask_ui\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nagasudhir\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D5A464-072F-400A-9B08-527BDFFDBC86}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="9555" windowHeight="8010"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="35">
   <si>
     <t>flaskSecret</t>
   </si>
@@ -126,12 +127,15 @@
   </si>
   <si>
     <t>/mis_dashboard</t>
+  </si>
+  <si>
+    <t>monthlyReportsFolderPath</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -203,7 +207,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -295,6 +299,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -330,6 +351,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -505,11 +543,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -712,46 +750,54 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1"/>
-    <hyperlink ref="B6" r:id="rId2"/>
-    <hyperlink ref="B7" r:id="rId3"/>
-    <hyperlink ref="B8" r:id="rId4"/>
-    <hyperlink ref="B9" r:id="rId5"/>
-    <hyperlink ref="B10" r:id="rId6"/>
-    <hyperlink ref="B11" r:id="rId7"/>
-    <hyperlink ref="B12" r:id="rId8"/>
-    <hyperlink ref="B13:B16" r:id="rId9" display="http://google.com"/>
-    <hyperlink ref="B17" r:id="rId10"/>
-    <hyperlink ref="B19" r:id="rId11"/>
-    <hyperlink ref="B20" r:id="rId12"/>
-    <hyperlink ref="B22" r:id="rId13"/>
-    <hyperlink ref="B23:B24" r:id="rId14" display="http://google.com"/>
-    <hyperlink ref="B21" r:id="rId15"/>
-    <hyperlink ref="B27" r:id="rId16"/>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B6" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B7" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B8" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B9" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B10" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B11" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B12" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B13:B16" r:id="rId9" display="http://google.com" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B17" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B19" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B20" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B22" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B23:B24" r:id="rId14" display="http://google.com" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B21" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B28" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId17"/>
@@ -759,7 +805,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -771,7 +817,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>